<commit_message>
mod @20171223 by yxq
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Vehicles.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Vehicles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="18528" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="“Vehicles” Settings" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>ID</t>
   </si>
@@ -133,16 +133,28 @@
     <t>NA</t>
   </si>
   <si>
+    <t>货车1</t>
+  </si>
+  <si>
     <t>货车</t>
   </si>
   <si>
     <t>hire</t>
   </si>
   <si>
+    <t>百度1</t>
+  </si>
+  <si>
     <t>百度</t>
   </si>
   <si>
+    <t>滴滴1</t>
+  </si>
+  <si>
     <t>滴滴</t>
+  </si>
+  <si>
+    <t>货车2</t>
   </si>
 </sst>
 </file>
@@ -150,10 +162,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -172,6 +184,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -180,6 +222,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -188,39 +292,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,14 +315,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,67 +327,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -325,37 +337,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,145 +487,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,6 +598,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -603,8 +654,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -634,21 +687,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -657,177 +695,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1174,50 +1186,50 @@
   <sheetPr/>
   <dimension ref="A1:AQ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <cols>
-    <col min="2" max="2" width="13.425" customWidth="1"/>
-    <col min="3" max="3" width="20.2833333333333" customWidth="1"/>
-    <col min="4" max="4" width="16.8583333333333" customWidth="1"/>
-    <col min="5" max="5" width="15.2833333333333" customWidth="1"/>
-    <col min="6" max="6" width="14.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="15.7083333333333" customWidth="1"/>
-    <col min="8" max="8" width="22.7083333333333" customWidth="1"/>
+    <col min="2" max="2" width="15.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="20.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="16.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="14.5648148148148" customWidth="1"/>
+    <col min="7" max="7" width="15.7037037037037" customWidth="1"/>
+    <col min="8" max="8" width="22.712962962963" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="25.1416666666667" customWidth="1"/>
+    <col min="10" max="10" width="25.1388888888889" customWidth="1"/>
     <col min="11" max="11" width="33" customWidth="1"/>
-    <col min="12" max="12" width="12.5666666666667" customWidth="1"/>
+    <col min="12" max="12" width="12.5648148148148" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="15" width="10.7083333333333" customWidth="1"/>
-    <col min="16" max="16" width="13.2833333333333" customWidth="1"/>
-    <col min="17" max="17" width="12.2833333333333" customWidth="1"/>
-    <col min="18" max="18" width="14.1416666666667" customWidth="1"/>
-    <col min="19" max="19" width="10.7083333333333" customWidth="1"/>
-    <col min="20" max="20" width="6.85833333333333" customWidth="1"/>
-    <col min="21" max="21" width="13.2833333333333" customWidth="1"/>
-    <col min="22" max="22" width="12.2833333333333" customWidth="1"/>
-    <col min="23" max="23" width="14.1416666666667" customWidth="1"/>
-    <col min="24" max="24" width="6.85833333333333" customWidth="1"/>
+    <col min="14" max="15" width="10.7037037037037" customWidth="1"/>
+    <col min="16" max="16" width="13.287037037037" customWidth="1"/>
+    <col min="17" max="17" width="12.287037037037" customWidth="1"/>
+    <col min="18" max="18" width="14.1388888888889" customWidth="1"/>
+    <col min="19" max="19" width="10.7037037037037" customWidth="1"/>
+    <col min="20" max="20" width="6.86111111111111" customWidth="1"/>
+    <col min="21" max="21" width="13.287037037037" customWidth="1"/>
+    <col min="22" max="22" width="12.287037037037" customWidth="1"/>
+    <col min="23" max="23" width="14.1388888888889" customWidth="1"/>
+    <col min="24" max="24" width="6.86111111111111" customWidth="1"/>
     <col min="25" max="25" width="6" customWidth="1"/>
-    <col min="26" max="26" width="13.2833333333333" customWidth="1"/>
-    <col min="27" max="27" width="12.2833333333333" customWidth="1"/>
-    <col min="28" max="28" width="14.1416666666667" customWidth="1"/>
+    <col min="26" max="26" width="13.287037037037" customWidth="1"/>
+    <col min="27" max="27" width="12.287037037037" customWidth="1"/>
+    <col min="28" max="28" width="14.1388888888889" customWidth="1"/>
     <col min="29" max="29" width="6" customWidth="1"/>
-    <col min="30" max="30" width="10.7083333333333" customWidth="1"/>
-    <col min="31" max="31" width="13.2833333333333" customWidth="1"/>
-    <col min="32" max="32" width="12.2833333333333" customWidth="1"/>
-    <col min="33" max="33" width="14.1416666666667" customWidth="1"/>
-    <col min="34" max="35" width="10.7083333333333" customWidth="1"/>
-    <col min="36" max="36" width="13.2833333333333" customWidth="1"/>
-    <col min="37" max="37" width="12.2833333333333" customWidth="1"/>
-    <col min="38" max="38" width="14.1416666666667" customWidth="1"/>
-    <col min="41" max="41" width="13.2833333333333" customWidth="1"/>
-    <col min="42" max="42" width="12.2833333333333" customWidth="1"/>
-    <col min="43" max="43" width="14.1416666666667" customWidth="1"/>
+    <col min="30" max="30" width="10.7037037037037" customWidth="1"/>
+    <col min="31" max="31" width="13.287037037037" customWidth="1"/>
+    <col min="32" max="32" width="12.287037037037" customWidth="1"/>
+    <col min="33" max="33" width="14.1388888888889" customWidth="1"/>
+    <col min="34" max="35" width="10.7037037037037" customWidth="1"/>
+    <col min="36" max="36" width="13.287037037037" customWidth="1"/>
+    <col min="37" max="37" width="12.287037037037" customWidth="1"/>
+    <col min="38" max="38" width="14.1388888888889" customWidth="1"/>
+    <col min="41" max="41" width="13.287037037037" customWidth="1"/>
+    <col min="42" max="42" width="12.287037037037" customWidth="1"/>
+    <col min="43" max="43" width="14.1388888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -1404,13 +1416,13 @@
         <v>39</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6">
         <v>400</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F3" s="6">
         <v>20</v>
@@ -1478,16 +1490,16 @@
         <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D4" s="6">
         <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" s="6">
         <v>12</v>
@@ -1555,16 +1567,16 @@
         <v>38</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" s="6">
         <v>60</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6">
         <v>20</v>
@@ -1640,16 +1652,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6">
         <v>400</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6">
         <v>20</v>

</xml_diff>

<commit_message>
mod @20171227 by yxq
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Vehicles.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Vehicles.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19104" windowHeight="7787"/>
+    <workbookView windowWidth="18528" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="“Vehicles” Settings" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>ID</t>
   </si>
@@ -25,7 +25,7 @@
     <t>vehicle weight limit *</t>
   </si>
   <si>
-    <t>maximum load</t>
+    <t>vehicle quantity</t>
   </si>
   <si>
     <t>vehicle source *</t>
@@ -73,13 +73,13 @@
     <t>distance interval 6</t>
   </si>
   <si>
-    <t>&lt;10km</t>
-  </si>
-  <si>
-    <t>10km-30km</t>
-  </si>
-  <si>
-    <t>&gt;30km</t>
+    <t xml:space="preserve">≤10km </t>
+  </si>
+  <si>
+    <t>&gt;10km,≤30km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;30km </t>
   </si>
   <si>
     <t>(0,a] km</t>
@@ -148,10 +148,13 @@
     <t>hire</t>
   </si>
   <si>
+    <t>滴滴</t>
+  </si>
+  <si>
     <t>百度</t>
   </si>
   <si>
-    <t>滴滴</t>
+    <t>达达</t>
   </si>
 </sst>
 </file>
@@ -159,10 +162,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -519,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -531,89 +534,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -732,7 +652,7 @@
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -762,7 +682,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -780,28 +700,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -810,10 +730,10 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -871,37 +791,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1221,52 +1124,55 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <cols>
-    <col min="2" max="2" width="15.8333333333333" customWidth="1"/>
-    <col min="3" max="3" width="20.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="16.8611111111111" customWidth="1"/>
-    <col min="5" max="5" width="15.287037037037" customWidth="1"/>
-    <col min="6" max="8" width="14.5648148148148" customWidth="1"/>
-    <col min="9" max="9" width="15.7037037037037" customWidth="1"/>
-    <col min="10" max="10" width="22.712962962963" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="25.1388888888889" customWidth="1"/>
-    <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="14" width="12.5648148148148" customWidth="1"/>
+    <col min="1" max="1" width="3.85185185185185" customWidth="1"/>
+    <col min="2" max="2" width="16.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.712962962963" customWidth="1"/>
+    <col min="4" max="4" width="14.8518518518519" customWidth="1"/>
+    <col min="5" max="5" width="15.5740740740741" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="14.712962962963" customWidth="1"/>
+    <col min="8" max="8" width="11.5740740740741" customWidth="1"/>
+    <col min="9" max="9" width="16.4259259259259" customWidth="1"/>
+    <col min="10" max="10" width="23.5740740740741" customWidth="1"/>
+    <col min="11" max="11" width="20.712962962963" customWidth="1"/>
+    <col min="12" max="12" width="25.712962962963" customWidth="1"/>
+    <col min="13" max="13" width="33.4259259259259" customWidth="1"/>
+    <col min="14" max="14" width="12.8518518518519" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="17" width="10.7037037037037" customWidth="1"/>
-    <col min="18" max="18" width="13.287037037037" customWidth="1"/>
-    <col min="19" max="19" width="12.287037037037" customWidth="1"/>
-    <col min="20" max="20" width="14.1388888888889" customWidth="1"/>
-    <col min="21" max="21" width="10.7037037037037" customWidth="1"/>
-    <col min="22" max="22" width="6.86111111111111" customWidth="1"/>
-    <col min="23" max="23" width="13.287037037037" customWidth="1"/>
-    <col min="24" max="24" width="12.287037037037" customWidth="1"/>
-    <col min="25" max="25" width="14.1388888888889" customWidth="1"/>
-    <col min="26" max="26" width="6.86111111111111" customWidth="1"/>
-    <col min="27" max="27" width="6" customWidth="1"/>
-    <col min="28" max="28" width="13.287037037037" customWidth="1"/>
-    <col min="29" max="29" width="12.287037037037" customWidth="1"/>
-    <col min="30" max="30" width="14.1388888888889" customWidth="1"/>
-    <col min="31" max="31" width="6" customWidth="1"/>
-    <col min="32" max="32" width="10.7037037037037" customWidth="1"/>
-    <col min="33" max="33" width="13.287037037037" customWidth="1"/>
-    <col min="34" max="34" width="12.287037037037" customWidth="1"/>
-    <col min="35" max="35" width="14.1388888888889" customWidth="1"/>
-    <col min="36" max="37" width="10.7037037037037" customWidth="1"/>
-    <col min="38" max="38" width="13.287037037037" customWidth="1"/>
-    <col min="39" max="39" width="12.287037037037" customWidth="1"/>
-    <col min="40" max="40" width="14.1388888888889" customWidth="1"/>
-    <col min="43" max="43" width="13.287037037037" customWidth="1"/>
-    <col min="44" max="44" width="12.287037037037" customWidth="1"/>
-    <col min="45" max="45" width="14.1388888888889" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.5740740740741" customWidth="1"/>
+    <col min="18" max="18" width="13.4259259259259" customWidth="1"/>
+    <col min="19" max="19" width="12.8518518518519" customWidth="1"/>
+    <col min="20" max="20" width="14.5740740740741" customWidth="1"/>
+    <col min="21" max="22" width="12.8518518518519" customWidth="1"/>
+    <col min="23" max="23" width="13.4259259259259" customWidth="1"/>
+    <col min="24" max="24" width="12.8518518518519" customWidth="1"/>
+    <col min="25" max="25" width="14.5740740740741" customWidth="1"/>
+    <col min="26" max="26" width="11.4259259259259" customWidth="1"/>
+    <col min="27" max="27" width="10.5740740740741" customWidth="1"/>
+    <col min="28" max="28" width="13.4259259259259" customWidth="1"/>
+    <col min="29" max="29" width="12.8518518518519" customWidth="1"/>
+    <col min="30" max="30" width="14.5740740740741" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="10.712962962963" customWidth="1"/>
+    <col min="33" max="33" width="13.4259259259259" customWidth="1"/>
+    <col min="34" max="34" width="12.8518518518519" customWidth="1"/>
+    <col min="35" max="35" width="14.5740740740741" customWidth="1"/>
+    <col min="36" max="37" width="10.712962962963" customWidth="1"/>
+    <col min="38" max="38" width="13.4259259259259" customWidth="1"/>
+    <col min="39" max="39" width="12.8518518518519" customWidth="1"/>
+    <col min="40" max="40" width="14.5740740740741" customWidth="1"/>
+    <col min="43" max="43" width="13.4259259259259" customWidth="1"/>
+    <col min="44" max="44" width="12.8518518518519" customWidth="1"/>
+    <col min="45" max="45" width="14.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45">
@@ -1279,17 +1185,17 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1305,412 +1211,495 @@
       <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10" t="s">
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10" t="s">
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10" t="s">
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10" t="s">
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="11" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12" t="s">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="V2" s="2"/>
+      <c r="W2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Z2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12" t="s">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AE2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12" t="s">
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AH2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="13" t="s">
+      <c r="AI2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12" t="s">
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AM2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN2" s="13" t="s">
+      <c r="AN2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AO2" s="11" t="s">
+      <c r="AO2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12" t="s">
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AR2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="13" t="s">
+      <c r="AS2" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:45">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="9">
-        <v>400</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="5">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <v>15</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <v>20</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="5">
         <v>30</v>
       </c>
-      <c r="I3" s="9">
-        <v>99999</v>
-      </c>
-      <c r="J3" s="9">
-        <v>99999</v>
-      </c>
-      <c r="K3" s="9">
-        <v>99999</v>
-      </c>
-      <c r="L3" s="9">
-        <v>400</v>
-      </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9">
+      <c r="I3" s="5">
+        <v>99</v>
+      </c>
+      <c r="J3" s="5">
+        <v>999</v>
+      </c>
+      <c r="K3" s="5">
+        <v>999</v>
+      </c>
+      <c r="L3" s="5">
+        <v>999</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5">
         <v>0</v>
       </c>
-      <c r="Q3" s="9">
-        <v>5</v>
-      </c>
-      <c r="R3" s="9">
-        <v>30</v>
-      </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9">
-        <v>5</v>
-      </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="9">
+      <c r="Q3" s="5">
         <v>0</v>
       </c>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
-      <c r="AM3" s="9"/>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="9"/>
-      <c r="AP3" s="9"/>
-      <c r="AQ3" s="9"/>
-      <c r="AR3" s="9"/>
-      <c r="AS3" s="9"/>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>999</v>
+      </c>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
     </row>
     <row r="4" spans="1:45">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="9">
-        <v>35</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="5">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <v>15</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <v>20</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="5">
         <v>30</v>
       </c>
-      <c r="I4" s="9">
-        <v>99999</v>
-      </c>
-      <c r="J4" s="9">
-        <v>5</v>
-      </c>
-      <c r="K4" s="9">
-        <v>99999</v>
-      </c>
-      <c r="L4" s="9">
-        <v>35</v>
-      </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9">
+      <c r="I4" s="5">
+        <v>99</v>
+      </c>
+      <c r="J4" s="5">
+        <v>999</v>
+      </c>
+      <c r="K4" s="5">
+        <v>999</v>
+      </c>
+      <c r="L4" s="5">
+        <v>999</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5">
         <v>0</v>
       </c>
-      <c r="Q4" s="9">
-        <v>5</v>
-      </c>
-      <c r="R4" s="9">
-        <v>11</v>
-      </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9">
-        <v>5</v>
-      </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9">
+      <c r="Q4" s="5">
         <v>0</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="R4" s="5">
+        <v>13</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5">
         <v>0</v>
       </c>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9"/>
+      <c r="V4" s="5">
+        <v>12</v>
+      </c>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>999</v>
+      </c>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
     </row>
     <row r="5" spans="1:45">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="9">
-        <v>60</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5">
+        <v>99</v>
+      </c>
+      <c r="J5" s="8">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>999</v>
+      </c>
+      <c r="L5" s="5">
+        <v>999</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>5</v>
+      </c>
+      <c r="R5" s="5">
+        <v>11</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+    </row>
+    <row r="6" spans="1:45">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5">
         <v>15</v>
       </c>
-      <c r="G5" s="9">
-        <v>20</v>
-      </c>
-      <c r="H5" s="9">
-        <v>30</v>
-      </c>
-      <c r="I5" s="9">
-        <v>99999</v>
-      </c>
-      <c r="J5" s="9">
-        <v>99999</v>
-      </c>
-      <c r="K5" s="9">
-        <v>99999</v>
-      </c>
-      <c r="L5" s="9">
-        <v>60</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9">
+      <c r="E6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="5">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6">
+        <v>99</v>
+      </c>
+      <c r="J6" s="8">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6">
+        <v>999</v>
+      </c>
+      <c r="L6" s="6">
+        <v>999</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5">
         <v>0</v>
       </c>
-      <c r="Q5" s="9">
-        <v>4</v>
-      </c>
-      <c r="R5" s="9">
-        <v>8</v>
-      </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9">
-        <v>4</v>
-      </c>
-      <c r="V5" s="9">
-        <v>15</v>
-      </c>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9">
+      <c r="Q6" s="5">
         <v>2</v>
       </c>
-      <c r="Y5" s="9">
-        <v>0.55</v>
-      </c>
-      <c r="Z5" s="9">
-        <v>15</v>
-      </c>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9">
-        <v>15</v>
-      </c>
-      <c r="AD5" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
+      <c r="R6" s="5">
+        <v>10</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5">
+        <v>2</v>
+      </c>
+      <c r="V6" s="5">
+        <v>10</v>
+      </c>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1741,7 +1730,7 @@
     <mergeCell ref="O1:O2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E4:E5 E6:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
       <formula1>"hire,own"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S6:S1048576">

</xml_diff>